<commit_message>
put .png maps (aq and distance to fire) into folder and re-knit .Rmd
</commit_message>
<xml_diff>
--- a/data/sitedata.xlsx
+++ b/data/sitedata.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,24 +8,24 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jordan Wingenroth\Documents\ucce_sonoma\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7507ED9E-CE97-4CDF-A40D-16AF5C3927D9}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B7D6F5D-B1DE-4F23-BA68-95F49F794809}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10275" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10275" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="all" sheetId="1" r:id="rId1"/>
     <sheet name="complete" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all!$A$1:$J$25</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">all!$A$1:$G$25</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">complete!$A$1:$Q$31</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="62">
   <si>
     <t>Key</t>
   </si>
@@ -202,12 +202,21 @@
   </si>
   <si>
     <t>RANK:</t>
+  </si>
+  <si>
+    <t>distance</t>
+  </si>
+  <si>
+    <t>distance to perimeter of fire + urban area overlap</t>
+  </si>
+  <si>
+    <t>local sensors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -685,8 +694,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1041,30 +1051,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView zoomScale="103" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" zoomScale="103" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2:M25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="45.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="21.85546875" customWidth="1"/>
-    <col min="14" max="14" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1084,1387 +1091,1039 @@
         <v>5</v>
       </c>
       <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" t="s">
+        <v>58</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L1" t="s">
+        <v>9</v>
+      </c>
+      <c r="M1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="1">
+        <v>38.504246999999999</v>
+      </c>
+      <c r="D2" s="1">
+        <v>-122.762199</v>
+      </c>
+      <c r="E2" s="1">
+        <v>0.57195571999999995</v>
+      </c>
+      <c r="F2" s="1">
+        <v>0.66720296599999995</v>
+      </c>
+      <c r="G2" s="1">
+        <v>0.81138388242761605</v>
+      </c>
+      <c r="H2" s="1">
+        <v>1.1971011962005101E-2</v>
+      </c>
+      <c r="J2">
+        <f t="shared" ref="J2:J25" si="0">RANK(E2,E$2:E$25)</f>
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K2">
+        <f t="shared" ref="K2:K25" si="1">RANK(F2,F$2:F$25)</f>
+        <v>4</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:M25" si="2">RANK(G2,G$2:G$25)</f>
+        <v>23</v>
+      </c>
+      <c r="M2">
+        <f>RANK(H2,H$2:H$25,1)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>38.389173</v>
+      </c>
+      <c r="D3" s="1">
+        <v>-122.93165399999999</v>
+      </c>
+      <c r="E3" s="1">
+        <v>0.243542435</v>
+      </c>
+      <c r="F3" s="1">
+        <v>0.25620836299999999</v>
+      </c>
+      <c r="G3" s="1">
+        <v>0.92978725591212896</v>
+      </c>
+      <c r="H3" s="1">
+        <v>0.19448597408698801</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="1"/>
+        <v>24</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="2"/>
+        <v>13</v>
+      </c>
+      <c r="M3">
+        <f t="shared" ref="M3:M25" si="3">RANK(H3,H$2:H$25,1)</f>
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="1">
+        <v>38.278485000000003</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-122.661661</v>
+      </c>
+      <c r="E4" s="1">
+        <v>0.49815498200000002</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0.51997869399999996</v>
+      </c>
+      <c r="G4" s="1">
+        <v>0.94554571947024701</v>
+      </c>
+      <c r="H4" s="1">
+        <v>0.14196961458607099</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="1"/>
+        <v>12</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="3"/>
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1">
+        <v>38.252895000000002</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-122.70068999999999</v>
+      </c>
+      <c r="E5" s="1">
+        <v>0.33210332100000001</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.35213930300000001</v>
+      </c>
+      <c r="G5" s="1">
+        <v>0.94460426054576996</v>
+      </c>
+      <c r="H5" s="1">
+        <v>0.17483700441043301</v>
+      </c>
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="1"/>
+        <v>22</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C6" s="1">
+        <v>38.246876</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-122.64398</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.49815498200000002</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.49885340099999997</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.934563693014834</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.15496399463057201</v>
+      </c>
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="3"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7" s="1">
+        <v>38.261111</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-122.642107</v>
+      </c>
+      <c r="E7" s="1">
+        <v>0.49815498200000002</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0.51787430000000001</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.93677498396412795</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.144123440494592</v>
+      </c>
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="1"/>
+        <v>13</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="3"/>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1">
+        <v>38.324100000000001</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-122.69032</v>
+      </c>
+      <c r="E8" s="1">
+        <v>0.49815498200000002</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0.52388457899999996</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0.99047514291911398</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.10436006881146601</v>
+      </c>
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="3"/>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C9" s="1">
+        <v>38.324818</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-122.69176</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0.49815498200000002</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0.52388457899999996</v>
+      </c>
+      <c r="G9" s="1">
+        <v>1</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0.104285361679869</v>
+      </c>
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="3"/>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1">
+        <v>38.404736</v>
+      </c>
+      <c r="D10" s="1">
+        <v>-122.83999</v>
+      </c>
+      <c r="E10" s="1">
+        <v>0.413284133</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0.41489698899999999</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0.94751581682763197</v>
+      </c>
+      <c r="H10" s="1">
+        <v>0.10790994225235701</v>
+      </c>
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="3"/>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="1">
+        <v>38.372486000000002</v>
+      </c>
+      <c r="D11" s="1">
+        <v>-122.79931000000001</v>
+      </c>
+      <c r="E11" s="1">
+        <v>0.413284133</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0.41199847899999997</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.94492949790061198</v>
+      </c>
+      <c r="H11" s="1">
+        <v>0.107182505077898</v>
+      </c>
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="1"/>
+        <v>20</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="3"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>40</v>
+      </c>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="1">
+        <v>38.400170000000003</v>
+      </c>
+      <c r="D12" s="1">
+        <v>-122.828064</v>
+      </c>
+      <c r="E12" s="1">
+        <v>0.413284133</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0.41966617299999998</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0.94984115085023901</v>
+      </c>
+      <c r="H12" s="1">
+        <v>0.101680714007489</v>
+      </c>
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="3"/>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="1">
+        <v>38.386102000000001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>-122.801047</v>
+      </c>
+      <c r="E13" s="1">
+        <v>0.413284133</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0.42847022099999998</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.94539557869122604</v>
+      </c>
+      <c r="H13" s="1">
+        <v>9.5888515663964002E-2</v>
+      </c>
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="1"/>
+        <v>17</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>58</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="M13">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" t="s">
+        <v>47</v>
+      </c>
+      <c r="C14" s="1">
+        <v>38.402251999999997</v>
+      </c>
+      <c r="D14" s="1">
+        <v>-122.83709</v>
+      </c>
+      <c r="E14" s="1">
+        <v>0.413284133</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0.40963906700000002</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0.94751581682763197</v>
+      </c>
+      <c r="H14" s="1">
+        <v>0.107143851436572</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="1"/>
+        <v>21</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="M1" t="s">
-        <v>5</v>
-      </c>
-      <c r="N1" t="s">
-        <v>6</v>
-      </c>
-      <c r="O1" t="s">
-        <v>7</v>
-      </c>
-      <c r="P1" t="s">
-        <v>8</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2">
-        <v>38.324818</v>
-      </c>
-      <c r="D2">
-        <v>-122.69176</v>
-      </c>
-      <c r="E2">
-        <v>0.49815498200000002</v>
-      </c>
-      <c r="F2">
-        <v>0.52388457899999996</v>
-      </c>
-      <c r="G2">
-        <v>0.87305871785912104</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2">
-        <v>0.88361504655352996</v>
-      </c>
-      <c r="J2">
-        <v>1</v>
-      </c>
-      <c r="L2">
-        <f>RANK(E2,E$2:E$25)</f>
-        <v>9</v>
-      </c>
-      <c r="M2">
-        <f>RANK(F2,F$2:F$25)</f>
-        <v>10</v>
-      </c>
-      <c r="N2">
-        <f>RANK(G2,G$2:G$25)</f>
-        <v>6</v>
-      </c>
-      <c r="O2">
-        <f>RANK(H2,H$2:H$25)</f>
-        <v>1</v>
-      </c>
-      <c r="P2">
-        <f>RANK(I2,I$2:I$25)</f>
-        <v>6</v>
-      </c>
-      <c r="Q2">
-        <f>RANK(J2,J$2:J$25)</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C3">
-        <v>38.324100000000001</v>
-      </c>
-      <c r="D3">
-        <v>-122.69032</v>
-      </c>
-      <c r="E3">
-        <v>0.49815498200000002</v>
-      </c>
-      <c r="F3">
-        <v>0.52388457899999996</v>
-      </c>
-      <c r="G3">
-        <v>0.87958476614799697</v>
-      </c>
-      <c r="H3">
-        <v>0.98901438769974204</v>
-      </c>
-      <c r="I3">
-        <v>0.89247115812323796</v>
-      </c>
-      <c r="J3">
-        <v>0.99047514291911398</v>
-      </c>
-      <c r="L3">
-        <f>RANK(E3,E$2:E$25)</f>
-        <v>9</v>
-      </c>
-      <c r="M3">
-        <f>RANK(F3,F$2:F$25)</f>
-        <v>10</v>
-      </c>
-      <c r="N3">
-        <f>RANK(G3,G$2:G$25)</f>
-        <v>5</v>
-      </c>
-      <c r="O3">
-        <f>RANK(H3,H$2:H$25)</f>
-        <v>2</v>
-      </c>
-      <c r="P3">
-        <f>RANK(I3,I$2:I$25)</f>
-        <v>5</v>
-      </c>
-      <c r="Q3">
-        <f>RANK(J3,J$2:J$25)</f>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" t="s">
-        <v>41</v>
-      </c>
-      <c r="C4">
-        <v>38.400170000000003</v>
-      </c>
-      <c r="D4">
-        <v>-122.828064</v>
-      </c>
-      <c r="E4">
-        <v>0.413284133</v>
-      </c>
-      <c r="F4">
-        <v>0.41966617299999998</v>
-      </c>
-      <c r="G4">
-        <v>0.75947040420984002</v>
-      </c>
-      <c r="H4">
-        <v>0.97472663768304102</v>
-      </c>
-      <c r="I4">
-        <v>0.74850908500490498</v>
-      </c>
-      <c r="J4">
-        <v>0.94984115085023901</v>
-      </c>
-      <c r="L4">
-        <f>RANK(E4,E$2:E$25)</f>
-        <v>17</v>
-      </c>
-      <c r="M4">
-        <f>RANK(F4,F$2:F$25)</f>
-        <v>18</v>
-      </c>
-      <c r="N4">
-        <f>RANK(G4,G$2:G$25)</f>
-        <v>12</v>
-      </c>
-      <c r="O4">
-        <f>RANK(H4,H$2:H$25)</f>
-        <v>3</v>
-      </c>
-      <c r="P4">
-        <f>RANK(I4,I$2:I$25)</f>
-        <v>21</v>
-      </c>
-      <c r="Q4">
-        <f>RANK(J4,J$2:J$25)</f>
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5">
-        <v>38.404736</v>
-      </c>
-      <c r="D5">
-        <v>-122.83999</v>
-      </c>
-      <c r="E5">
-        <v>0.413284133</v>
-      </c>
-      <c r="F5">
-        <v>0.41489698899999999</v>
-      </c>
-      <c r="G5">
-        <v>0.76118373629429203</v>
-      </c>
-      <c r="H5">
-        <v>0.96992651141031605</v>
-      </c>
-      <c r="I5">
-        <v>0.75327567160079001</v>
-      </c>
-      <c r="J5">
-        <v>0.94751581682763197</v>
-      </c>
-      <c r="L5">
-        <f>RANK(E5,E$2:E$25)</f>
-        <v>17</v>
-      </c>
-      <c r="M5">
-        <f>RANK(F5,F$2:F$25)</f>
-        <v>19</v>
-      </c>
-      <c r="N5">
-        <f>RANK(G5,G$2:G$25)</f>
-        <v>10</v>
-      </c>
-      <c r="O5">
-        <f>RANK(H5,H$2:H$25)</f>
-        <v>4</v>
-      </c>
-      <c r="P5">
-        <f>RANK(I5,I$2:I$25)</f>
-        <v>19</v>
-      </c>
-      <c r="Q5">
-        <f>RANK(J5,J$2:J$25)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6">
-        <v>38.402251999999997</v>
-      </c>
-      <c r="D6">
-        <v>-122.83709</v>
-      </c>
-      <c r="E6">
-        <v>0.413284133</v>
-      </c>
-      <c r="F6">
-        <v>0.40963906700000002</v>
-      </c>
-      <c r="G6">
-        <v>0.76118373629429203</v>
-      </c>
-      <c r="H6">
-        <v>0.96992651141031605</v>
-      </c>
-      <c r="I6">
-        <v>0.75327567160079001</v>
-      </c>
-      <c r="J6">
-        <v>0.94751581682763197</v>
-      </c>
-      <c r="L6">
-        <f>RANK(E6,E$2:E$25)</f>
-        <v>17</v>
-      </c>
-      <c r="M6">
-        <f>RANK(F6,F$2:F$25)</f>
-        <v>21</v>
-      </c>
-      <c r="N6">
-        <f>RANK(G6,G$2:G$25)</f>
-        <v>10</v>
-      </c>
-      <c r="O6">
-        <f>RANK(H6,H$2:H$25)</f>
-        <v>4</v>
-      </c>
-      <c r="P6">
-        <f>RANK(I6,I$2:I$25)</f>
-        <v>19</v>
-      </c>
-      <c r="Q6">
-        <f>RANK(J6,J$2:J$25)</f>
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="M14">
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7">
-        <v>38.278485000000003</v>
-      </c>
-      <c r="D7">
-        <v>-122.661661</v>
-      </c>
-      <c r="E7">
-        <v>0.49815498200000002</v>
-      </c>
-      <c r="F7">
-        <v>0.51997869399999996</v>
-      </c>
-      <c r="G7">
-        <v>0.94998330764139804</v>
-      </c>
-      <c r="H7">
-        <v>0.93541027363785501</v>
-      </c>
-      <c r="I7">
-        <v>0.97000411712301604</v>
-      </c>
-      <c r="J7">
-        <v>0.94554571947024701</v>
-      </c>
-      <c r="L7">
-        <f>RANK(E7,E$2:E$25)</f>
-        <v>9</v>
-      </c>
-      <c r="M7">
-        <f>RANK(F7,F$2:F$25)</f>
-        <v>12</v>
-      </c>
-      <c r="N7">
-        <f>RANK(G7,G$2:G$25)</f>
-        <v>3</v>
-      </c>
-      <c r="O7">
-        <f>RANK(H7,H$2:H$25)</f>
-        <v>10</v>
-      </c>
-      <c r="P7">
-        <f>RANK(I7,I$2:I$25)</f>
-        <v>3</v>
-      </c>
-      <c r="Q7">
-        <f>RANK(J7,J$2:J$25)</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B8" t="s">
-        <v>43</v>
-      </c>
-      <c r="C8">
-        <v>38.386102000000001</v>
-      </c>
-      <c r="D8">
-        <v>-122.801047</v>
-      </c>
-      <c r="E8">
-        <v>0.413284133</v>
-      </c>
-      <c r="F8">
-        <v>0.42847022099999998</v>
-      </c>
-      <c r="G8">
-        <v>0.76974779040043795</v>
-      </c>
-      <c r="H8">
-        <v>0.96328721301500797</v>
-      </c>
-      <c r="I8">
-        <v>0.77007003487992498</v>
-      </c>
-      <c r="J8">
-        <v>0.94539557869122604</v>
-      </c>
-      <c r="L8">
-        <f>RANK(E8,E$2:E$25)</f>
-        <v>17</v>
-      </c>
-      <c r="M8">
-        <f>RANK(F8,F$2:F$25)</f>
-        <v>17</v>
-      </c>
-      <c r="N8">
-        <f>RANK(G8,G$2:G$25)</f>
-        <v>9</v>
-      </c>
-      <c r="O8">
-        <f>RANK(H8,H$2:H$25)</f>
-        <v>6</v>
-      </c>
-      <c r="P8">
-        <f>RANK(I8,I$2:I$25)</f>
-        <v>14</v>
-      </c>
-      <c r="Q8">
-        <f>RANK(J8,J$2:J$25)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>35</v>
-      </c>
-      <c r="C9">
-        <v>38.372486000000002</v>
-      </c>
-      <c r="D9">
-        <v>-122.79931000000001</v>
-      </c>
-      <c r="E9">
-        <v>0.413284133</v>
-      </c>
-      <c r="F9">
-        <v>0.41199847899999997</v>
-      </c>
-      <c r="G9">
-        <v>0.77652689132332697</v>
-      </c>
-      <c r="H9">
-        <v>0.960293699554993</v>
-      </c>
-      <c r="I9">
-        <v>0.78069465425739204</v>
-      </c>
-      <c r="J9">
-        <v>0.94492949790061198</v>
-      </c>
-      <c r="L9">
-        <f>RANK(E9,E$2:E$25)</f>
-        <v>17</v>
-      </c>
-      <c r="M9">
-        <f>RANK(F9,F$2:F$25)</f>
-        <v>20</v>
-      </c>
-      <c r="N9">
-        <f>RANK(G9,G$2:G$25)</f>
-        <v>8</v>
-      </c>
-      <c r="O9">
-        <f>RANK(H9,H$2:H$25)</f>
-        <v>7</v>
-      </c>
-      <c r="P9">
-        <f>RANK(I9,I$2:I$25)</f>
-        <v>13</v>
-      </c>
-      <c r="Q9">
-        <f>RANK(J9,J$2:J$25)</f>
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10">
-        <v>38.252895000000002</v>
-      </c>
-      <c r="D10">
-        <v>-122.70068999999999</v>
-      </c>
-      <c r="E10">
-        <v>0.33210332100000001</v>
-      </c>
-      <c r="F10">
-        <v>0.35213930300000001</v>
-      </c>
-      <c r="G10">
-        <v>0.93525950037833405</v>
-      </c>
-      <c r="H10">
-        <v>0.93663534537036397</v>
-      </c>
-      <c r="I10">
-        <v>0.95322768849230599</v>
-      </c>
-      <c r="J10">
-        <v>0.94460426054576996</v>
-      </c>
-      <c r="L10">
-        <f>RANK(E10,E$2:E$25)</f>
-        <v>22</v>
-      </c>
-      <c r="M10">
-        <f>RANK(F10,F$2:F$25)</f>
-        <v>22</v>
-      </c>
-      <c r="N10">
-        <f>RANK(G10,G$2:G$25)</f>
-        <v>4</v>
-      </c>
-      <c r="O10">
-        <f>RANK(H10,H$2:H$25)</f>
-        <v>9</v>
-      </c>
-      <c r="P10">
-        <f>RANK(I10,I$2:I$25)</f>
-        <v>4</v>
-      </c>
-      <c r="Q10">
-        <f>RANK(J10,J$2:J$25)</f>
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>56</v>
-      </c>
-      <c r="B11" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11">
-        <v>38.261111</v>
-      </c>
-      <c r="D11">
-        <v>-122.642107</v>
-      </c>
-      <c r="E11">
-        <v>0.49815498200000002</v>
-      </c>
-      <c r="F11">
-        <v>0.51787430000000001</v>
-      </c>
-      <c r="G11">
-        <v>0.97058820712582194</v>
-      </c>
-      <c r="H11">
-        <v>0.92481623057247098</v>
-      </c>
-      <c r="I11">
-        <v>0.98545759088256302</v>
-      </c>
-      <c r="J11">
-        <v>0.93677498396412795</v>
-      </c>
-      <c r="L11">
-        <f>RANK(E11,E$2:E$25)</f>
-        <v>9</v>
-      </c>
-      <c r="M11">
-        <f>RANK(F11,F$2:F$25)</f>
-        <v>13</v>
-      </c>
-      <c r="N11">
-        <f>RANK(G11,G$2:G$25)</f>
-        <v>2</v>
-      </c>
-      <c r="O11">
-        <f>RANK(H11,H$2:H$25)</f>
-        <v>13</v>
-      </c>
-      <c r="P11">
-        <f>RANK(I11,I$2:I$25)</f>
-        <v>2</v>
-      </c>
-      <c r="Q11">
-        <f>RANK(J11,J$2:J$25)</f>
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>52</v>
-      </c>
-      <c r="B12" t="s">
-        <v>53</v>
-      </c>
-      <c r="C12">
-        <v>38.246876</v>
-      </c>
-      <c r="D12">
-        <v>-122.64398</v>
-      </c>
-      <c r="E12">
-        <v>0.49815498200000002</v>
-      </c>
-      <c r="F12">
-        <v>0.49885340099999997</v>
-      </c>
-      <c r="G12">
-        <v>0.97852272172935895</v>
-      </c>
-      <c r="H12">
-        <v>0.92230728407298102</v>
-      </c>
-      <c r="I12">
-        <v>0.99171893073483197</v>
-      </c>
-      <c r="J12">
-        <v>0.934563693014834</v>
-      </c>
-      <c r="L12">
-        <f>RANK(E12,E$2:E$25)</f>
-        <v>9</v>
-      </c>
-      <c r="M12">
-        <f>RANK(F12,F$2:F$25)</f>
-        <v>16</v>
-      </c>
-      <c r="N12">
-        <f>RANK(G12,G$2:G$25)</f>
-        <v>1</v>
-      </c>
-      <c r="O12">
-        <f>RANK(H12,H$2:H$25)</f>
-        <v>14</v>
-      </c>
-      <c r="P12">
-        <f>RANK(I12,I$2:I$25)</f>
-        <v>1</v>
-      </c>
-      <c r="Q12">
-        <f>RANK(J12,J$2:J$25)</f>
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B13" t="s">
-        <v>15</v>
-      </c>
-      <c r="C13">
-        <v>38.424272000000002</v>
-      </c>
-      <c r="D13">
-        <v>-122.795586</v>
-      </c>
-      <c r="E13">
-        <v>0.61254612500000005</v>
-      </c>
-      <c r="F13">
-        <v>0.56030041799999997</v>
-      </c>
-      <c r="G13">
-        <v>0.75297896409153597</v>
-      </c>
-      <c r="H13">
-        <v>0.94468937455606905</v>
-      </c>
-      <c r="I13">
-        <v>0.76289015791634596</v>
-      </c>
-      <c r="J13">
-        <v>0.93095890476514098</v>
-      </c>
-      <c r="L13">
-        <f>RANK(E13,E$2:E$25)</f>
-        <v>5</v>
-      </c>
-      <c r="M13">
-        <f>RANK(F13,F$2:F$25)</f>
-        <v>7</v>
-      </c>
-      <c r="N13">
-        <f>RANK(G13,G$2:G$25)</f>
-        <v>13</v>
-      </c>
-      <c r="O13">
-        <f>RANK(H13,H$2:H$25)</f>
-        <v>8</v>
-      </c>
-      <c r="P13">
-        <f>RANK(I13,I$2:I$25)</f>
-        <v>18</v>
-      </c>
-      <c r="Q13">
-        <f>RANK(J13,J$2:J$25)</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14" t="s">
-        <v>11</v>
-      </c>
-      <c r="C14">
-        <v>38.389173</v>
-      </c>
-      <c r="D14">
-        <v>-122.93165399999999</v>
-      </c>
-      <c r="E14">
-        <v>0.243542435</v>
-      </c>
-      <c r="F14">
-        <v>0.25620836299999999</v>
-      </c>
-      <c r="G14">
-        <v>0.71843207601737102</v>
-      </c>
-      <c r="H14">
-        <v>0.93518139820105395</v>
-      </c>
-      <c r="I14">
-        <v>0.74165744488096397</v>
-      </c>
-      <c r="J14">
-        <v>0.92978725591212896</v>
-      </c>
-      <c r="L14">
-        <f>RANK(E14,E$2:E$25)</f>
-        <v>24</v>
-      </c>
-      <c r="M14">
-        <f>RANK(F14,F$2:F$25)</f>
-        <v>24</v>
-      </c>
-      <c r="N14">
-        <f>RANK(G14,G$2:G$25)</f>
-        <v>15</v>
-      </c>
-      <c r="O14">
-        <f>RANK(H14,H$2:H$25)</f>
-        <v>11</v>
-      </c>
-      <c r="P14">
-        <f>RANK(I14,I$2:I$25)</f>
-        <v>22</v>
-      </c>
-      <c r="Q14">
-        <f>RANK(J14,J$2:J$25)</f>
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>54</v>
       </c>
       <c r="B15" t="s">
         <v>55</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="1">
         <v>38.443446999999999</v>
       </c>
-      <c r="D15">
+      <c r="D15" s="1">
         <v>-122.90854</v>
       </c>
-      <c r="E15">
+      <c r="E15" s="1">
         <v>0.273062731</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="1">
         <v>0.28880563999999997</v>
       </c>
-      <c r="G15">
-        <v>0.71125533666128304</v>
-      </c>
-      <c r="H15">
-        <v>0.92583945291548697</v>
-      </c>
-      <c r="I15">
-        <v>0.73983737326675303</v>
+      <c r="G15" s="1">
+        <v>0.922314295624169</v>
+      </c>
+      <c r="H15" s="1">
+        <v>0.15512798033163999</v>
       </c>
       <c r="J15">
-        <v>0.922314295624169</v>
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>23</v>
       </c>
       <c r="L15">
-        <f>RANK(E15,E$2:E$25)</f>
-        <v>23</v>
+        <f t="shared" si="2"/>
+        <v>14</v>
       </c>
       <c r="M15">
-        <f>RANK(F15,F$2:F$25)</f>
-        <v>23</v>
-      </c>
-      <c r="N15">
-        <f>RANK(G15,G$2:G$25)</f>
+        <f t="shared" si="3"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="1">
+        <v>38.424272000000002</v>
+      </c>
+      <c r="D16" s="1">
+        <v>-122.795586</v>
+      </c>
+      <c r="E16" s="1">
+        <v>0.61254612500000005</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0.56030041799999997</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0.93095890476514098</v>
+      </c>
+      <c r="H16" s="1">
+        <v>6.1649914548172702E-2</v>
+      </c>
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K16">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="3"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="1">
+        <v>38.460484000000001</v>
+      </c>
+      <c r="D17" s="1">
+        <v>-122.7204</v>
+      </c>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="1">
+        <v>1</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0.65272940808660596</v>
+      </c>
+      <c r="H17" s="1">
+        <v>1.04131903603931E-2</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="1">
+        <v>38.454853</v>
+      </c>
+      <c r="D18" s="1">
+        <v>-122.77546</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0.44280442800000003</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0.51122855499999997</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0.86020726910696399</v>
+      </c>
+      <c r="H18" s="1">
+        <v>2.6253845387480199E-2</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="1">
+        <v>38.463940000000001</v>
+      </c>
+      <c r="D19" s="1">
+        <v>-122.625114</v>
+      </c>
+      <c r="E19" s="1">
+        <v>0.80442804400000001</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0.64134004099999997</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0.86195571664569803</v>
+      </c>
+      <c r="H19" s="1">
+        <v>3.3314222503521097E-2</v>
+      </c>
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K19">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
-      <c r="O15">
-        <f>RANK(H15,H$2:H$25)</f>
-        <v>12</v>
-      </c>
-      <c r="P15">
-        <f>RANK(I15,I$2:I$25)</f>
-        <v>23</v>
-      </c>
-      <c r="Q15">
-        <f>RANK(J15,J$2:J$25)</f>
+      <c r="M19">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="1">
+        <v>38.448532</v>
+      </c>
+      <c r="D20" s="1">
+        <v>-122.76956</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0.44280442800000003</v>
+      </c>
+      <c r="F20" s="1">
+        <v>0.51573464099999999</v>
+      </c>
+      <c r="G20" s="1">
+        <v>0.87633037392801605</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2.62886174597689E-2</v>
+      </c>
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K20">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>16</v>
+      </c>
+      <c r="M20">
+        <f t="shared" si="3"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>36</v>
+      </c>
+      <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1">
+        <v>38.511105000000001</v>
+      </c>
+      <c r="D21" s="1">
+        <v>-122.77461</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0.57195571999999995</v>
+      </c>
+      <c r="F21" s="1">
+        <v>0.61325090500000001</v>
+      </c>
+      <c r="G21" s="1">
+        <v>0.83021673064214496</v>
+      </c>
+      <c r="H21" s="1">
+        <v>2.5480766672905199E-2</v>
+      </c>
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="K21">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="M21">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>38</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B22" t="s">
         <v>39</v>
       </c>
-      <c r="C16">
+      <c r="C22" s="1">
         <v>38.379387000000001</v>
       </c>
-      <c r="D16">
+      <c r="D22" s="1">
         <v>-122.7042</v>
       </c>
-      <c r="E16">
+      <c r="E22" s="1">
         <v>0.49815498200000002</v>
       </c>
-      <c r="F16">
+      <c r="F22" s="1">
         <v>0.554942343</v>
       </c>
-      <c r="G16">
-        <v>0.78090897205126597</v>
-      </c>
-      <c r="H16">
-        <v>0.89742618342444702</v>
-      </c>
-      <c r="I16">
-        <v>0.84023855804098102</v>
-      </c>
-      <c r="J16">
+      <c r="G22" s="1">
         <v>0.91117878510690797</v>
       </c>
-      <c r="L16">
-        <f>RANK(E16,E$2:E$25)</f>
+      <c r="H22" s="1">
+        <v>6.8558783647187205E-2</v>
+      </c>
+      <c r="J22">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="M16">
-        <f>RANK(F16,F$2:F$25)</f>
+      <c r="K22">
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
-      <c r="N16">
-        <f>RANK(G16,G$2:G$25)</f>
-        <v>7</v>
-      </c>
-      <c r="O16">
-        <f>RANK(H16,H$2:H$25)</f>
+      <c r="L22">
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
-      <c r="P16">
-        <f>RANK(I16,I$2:I$25)</f>
-        <v>8</v>
-      </c>
-      <c r="Q16">
-        <f>RANK(J16,J$2:J$25)</f>
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>32</v>
-      </c>
-      <c r="B17" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17">
-        <v>38.448532</v>
-      </c>
-      <c r="D17">
-        <v>-122.76956</v>
-      </c>
-      <c r="E17">
-        <v>0.44280442800000003</v>
-      </c>
-      <c r="F17">
-        <v>0.51573464099999999</v>
-      </c>
-      <c r="G17">
-        <v>0.71337529601660299</v>
-      </c>
-      <c r="H17">
-        <v>0.87022148723876502</v>
-      </c>
-      <c r="I17">
-        <v>0.76934371012906499</v>
-      </c>
-      <c r="J17">
-        <v>0.87633037392801605</v>
-      </c>
-      <c r="L17">
-        <f>RANK(E17,E$2:E$25)</f>
-        <v>15</v>
-      </c>
-      <c r="M17">
-        <f>RANK(F17,F$2:F$25)</f>
-        <v>14</v>
-      </c>
-      <c r="N17">
-        <f>RANK(G17,G$2:G$25)</f>
-        <v>16</v>
-      </c>
-      <c r="O17">
-        <f>RANK(H17,H$2:H$25)</f>
-        <v>16</v>
-      </c>
-      <c r="P17">
-        <f>RANK(I17,I$2:I$25)</f>
-        <v>15</v>
-      </c>
-      <c r="Q17">
-        <f>RANK(J17,J$2:J$25)</f>
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
-      <c r="C18">
-        <v>38.463940000000001</v>
-      </c>
-      <c r="D18">
-        <v>-122.625114</v>
-      </c>
-      <c r="E18">
-        <v>0.80442804400000001</v>
-      </c>
-      <c r="F18">
-        <v>0.64134004099999997</v>
-      </c>
-      <c r="G18">
-        <v>0.67042428106097995</v>
-      </c>
-      <c r="H18">
-        <v>0.78434001090357697</v>
-      </c>
-      <c r="I18">
-        <v>0.86053164146471395</v>
-      </c>
-      <c r="J18">
-        <v>0.86195571664569803</v>
-      </c>
-      <c r="L18">
-        <f>RANK(E18,E$2:E$25)</f>
-        <v>2</v>
-      </c>
-      <c r="M18">
-        <f>RANK(F18,F$2:F$25)</f>
-        <v>5</v>
-      </c>
-      <c r="N18">
-        <f>RANK(G18,G$2:G$25)</f>
-        <v>21</v>
-      </c>
-      <c r="O18">
-        <f>RANK(H18,H$2:H$25)</f>
-        <v>21</v>
-      </c>
-      <c r="P18">
-        <f>RANK(I18,I$2:I$25)</f>
-        <v>7</v>
-      </c>
-      <c r="Q18">
-        <f>RANK(J18,J$2:J$25)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>30</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19">
-        <v>38.552208</v>
-      </c>
-      <c r="D19">
-        <v>-122.80717</v>
-      </c>
-      <c r="E19">
-        <v>0.57195571999999995</v>
-      </c>
-      <c r="F19">
-        <v>0.52571819799999997</v>
-      </c>
-      <c r="G19">
-        <v>0.74084989829296</v>
-      </c>
-      <c r="H19">
-        <v>0.83547979293911401</v>
-      </c>
-      <c r="I19">
-        <v>0.83703997618506898</v>
-      </c>
-      <c r="J19">
-        <v>0.86188337820847605</v>
-      </c>
-      <c r="L19">
-        <f>RANK(E19,E$2:E$25)</f>
-        <v>6</v>
-      </c>
-      <c r="M19">
-        <f>RANK(F19,F$2:F$25)</f>
-        <v>9</v>
-      </c>
-      <c r="N19">
-        <f>RANK(G19,G$2:G$25)</f>
-        <v>14</v>
-      </c>
-      <c r="O19">
-        <f>RANK(H19,H$2:H$25)</f>
-        <v>19</v>
-      </c>
-      <c r="P19">
-        <f>RANK(I19,I$2:I$25)</f>
-        <v>9</v>
-      </c>
-      <c r="Q19">
-        <f>RANK(J19,J$2:J$25)</f>
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C20">
-        <v>38.454853</v>
-      </c>
-      <c r="D20">
-        <v>-122.77546</v>
-      </c>
-      <c r="E20">
-        <v>0.44280442800000003</v>
-      </c>
-      <c r="F20">
-        <v>0.51122855499999997</v>
-      </c>
-      <c r="G20">
-        <v>0.69999471408046998</v>
-      </c>
-      <c r="H20">
-        <v>0.84974435034155604</v>
-      </c>
-      <c r="I20">
-        <v>0.76701406550456297</v>
-      </c>
-      <c r="J20">
-        <v>0.86020726910696399</v>
-      </c>
-      <c r="L20">
-        <f>RANK(E20,E$2:E$25)</f>
-        <v>15</v>
-      </c>
-      <c r="M20">
-        <f>RANK(F20,F$2:F$25)</f>
-        <v>15</v>
-      </c>
-      <c r="N20">
-        <f>RANK(G20,G$2:G$25)</f>
-        <v>19</v>
-      </c>
-      <c r="O20">
-        <f>RANK(H20,H$2:H$25)</f>
-        <v>17</v>
-      </c>
-      <c r="P20">
-        <f>RANK(I20,I$2:I$25)</f>
-        <v>16</v>
-      </c>
-      <c r="Q20">
-        <f>RANK(J20,J$2:J$25)</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>50</v>
-      </c>
-      <c r="B21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21">
-        <v>38.420914000000003</v>
-      </c>
-      <c r="D21">
-        <v>-122.72789</v>
-      </c>
-      <c r="E21">
-        <v>0.66789667900000005</v>
-      </c>
-      <c r="F21">
-        <v>0.72485813300000002</v>
-      </c>
-      <c r="G21">
-        <v>0.70421405283124505</v>
-      </c>
-      <c r="H21">
-        <v>0.83980543379261696</v>
-      </c>
-      <c r="I21">
-        <v>0.78469910747978</v>
-      </c>
-      <c r="J21">
-        <v>0.85759943709418895</v>
-      </c>
-      <c r="L21">
-        <f>RANK(E21,E$2:E$25)</f>
-        <v>4</v>
-      </c>
-      <c r="M21">
-        <f>RANK(F21,F$2:F$25)</f>
-        <v>3</v>
-      </c>
-      <c r="N21">
-        <f>RANK(G21,G$2:G$25)</f>
-        <v>18</v>
-      </c>
-      <c r="O21">
-        <f>RANK(H21,H$2:H$25)</f>
-        <v>18</v>
-      </c>
-      <c r="P21">
-        <f>RANK(I21,I$2:I$25)</f>
-        <v>12</v>
-      </c>
-      <c r="Q21">
-        <f>RANK(J21,J$2:J$25)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>36</v>
-      </c>
-      <c r="B22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C22">
-        <v>38.511105000000001</v>
-      </c>
-      <c r="D22">
-        <v>-122.77461</v>
-      </c>
-      <c r="E22">
-        <v>0.57195571999999995</v>
-      </c>
-      <c r="F22">
-        <v>0.61325090500000001</v>
-      </c>
-      <c r="G22">
-        <v>0.68102661873182901</v>
-      </c>
-      <c r="H22">
-        <v>0.802774627825942</v>
-      </c>
-      <c r="I22">
-        <v>0.78497856288539902</v>
-      </c>
-      <c r="J22">
-        <v>0.83021673064214496</v>
-      </c>
-      <c r="L22">
-        <f>RANK(E22,E$2:E$25)</f>
-        <v>6</v>
-      </c>
       <c r="M22">
-        <f>RANK(F22,F$2:F$25)</f>
-        <v>6</v>
-      </c>
-      <c r="N22">
-        <f>RANK(G22,G$2:G$25)</f>
-        <v>20</v>
-      </c>
-      <c r="O22">
-        <f>RANK(H22,H$2:H$25)</f>
-        <v>20</v>
-      </c>
-      <c r="P22">
-        <f>RANK(I22,I$2:I$25)</f>
-        <v>11</v>
-      </c>
-      <c r="Q22">
-        <f>RANK(J22,J$2:J$25)</f>
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>48</v>
       </c>
       <c r="B23" t="s">
         <v>49</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="1">
         <v>38.438740000000003</v>
       </c>
-      <c r="D23">
+      <c r="D23" s="1">
         <v>-122.67097</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="1">
         <v>0.73062730600000003</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="1">
         <v>0.87509797199999995</v>
       </c>
-      <c r="G23">
-        <v>0.65147872389606498</v>
-      </c>
-      <c r="H23">
-        <v>0.77472269120845405</v>
-      </c>
-      <c r="I23">
-        <v>0.79222069059142297</v>
+      <c r="G23" s="1">
+        <v>0.82201958970682698</v>
+      </c>
+      <c r="H23" s="1">
+        <v>2.79411237719423E-2</v>
       </c>
       <c r="J23">
-        <v>0.82201958970682698</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="K23">
+        <f t="shared" si="1"/>
+        <v>2</v>
       </c>
       <c r="L23">
-        <f>RANK(E23,E$2:E$25)</f>
+        <f t="shared" si="2"/>
+        <v>22</v>
+      </c>
+      <c r="M23">
+        <f t="shared" si="3"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B24" t="s">
+        <v>51</v>
+      </c>
+      <c r="C24" s="1">
+        <v>38.420914000000003</v>
+      </c>
+      <c r="D24" s="1">
+        <v>-122.72789</v>
+      </c>
+      <c r="E24" s="1">
+        <v>0.66789667900000005</v>
+      </c>
+      <c r="F24" s="1">
+        <v>0.72485813300000002</v>
+      </c>
+      <c r="G24" s="1">
+        <v>0.85759943709418895</v>
+      </c>
+      <c r="H24" s="1">
+        <v>5.01192340658594E-2</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
-      <c r="M23">
-        <f>RANK(F23,F$2:F$25)</f>
-        <v>2</v>
-      </c>
-      <c r="N23">
-        <f>RANK(G23,G$2:G$25)</f>
-        <v>23</v>
-      </c>
-      <c r="O23">
-        <f>RANK(H23,H$2:H$25)</f>
-        <v>23</v>
-      </c>
-      <c r="P23">
-        <f>RANK(I23,I$2:I$25)</f>
-        <v>10</v>
-      </c>
-      <c r="Q23">
-        <f>RANK(J23,J$2:J$25)</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>12</v>
-      </c>
-      <c r="B24" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24">
-        <v>38.504246999999999</v>
-      </c>
-      <c r="D24">
-        <v>-122.762199</v>
-      </c>
-      <c r="E24">
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="M24">
+        <f t="shared" si="3"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" t="s">
+        <v>31</v>
+      </c>
+      <c r="C25" s="1">
+        <v>38.552208</v>
+      </c>
+      <c r="D25" s="1">
+        <v>-122.80717</v>
+      </c>
+      <c r="E25" s="1">
         <v>0.57195571999999995</v>
       </c>
-      <c r="F24">
-        <v>0.66720296599999995</v>
-      </c>
-      <c r="G24">
-        <v>0.65713424753857297</v>
-      </c>
-      <c r="H24">
-        <v>0.78292515898286197</v>
-      </c>
-      <c r="I24">
-        <v>0.76604683088717695</v>
-      </c>
-      <c r="J24">
-        <v>0.81138388242761605</v>
-      </c>
-      <c r="L24">
-        <f>RANK(E24,E$2:E$25)</f>
+      <c r="F25" s="1">
+        <v>0.52571819799999997</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.86188337820847605</v>
+      </c>
+      <c r="H25" s="1">
+        <v>7.1883961788163003E-2</v>
+      </c>
+      <c r="J25">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="M24">
-        <f>RANK(F24,F$2:F$25)</f>
-        <v>4</v>
-      </c>
-      <c r="N24">
-        <f>RANK(G24,G$2:G$25)</f>
-        <v>22</v>
-      </c>
-      <c r="O24">
-        <f>RANK(H24,H$2:H$25)</f>
-        <v>22</v>
-      </c>
-      <c r="P24">
-        <f>RANK(I24,I$2:I$25)</f>
-        <v>17</v>
-      </c>
-      <c r="Q24">
-        <f>RANK(J24,J$2:J$25)</f>
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="K25">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
-      <c r="B25" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25">
-        <v>38.460484000000001</v>
-      </c>
-      <c r="D25">
-        <v>-122.7204</v>
-      </c>
-      <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>1</v>
-      </c>
-      <c r="G25">
-        <v>0.50342463602194598</v>
-      </c>
-      <c r="H25">
-        <v>0.62943687236218204</v>
-      </c>
-      <c r="I25">
-        <v>0.626613713234349</v>
-      </c>
-      <c r="J25">
-        <v>0.65272940808660596</v>
-      </c>
-      <c r="L25">
-        <f>RANK(E25,E$2:E$25)</f>
-        <v>1</v>
-      </c>
       <c r="M25">
-        <f>RANK(F25,F$2:F$25)</f>
-        <v>1</v>
-      </c>
-      <c r="N25">
-        <f>RANK(G25,G$2:G$25)</f>
-        <v>24</v>
-      </c>
-      <c r="O25">
-        <f>RANK(H25,H$2:H$25)</f>
-        <v>24</v>
-      </c>
-      <c r="P25">
-        <f>RANK(I25,I$2:I$25)</f>
-        <v>24</v>
-      </c>
-      <c r="Q25">
-        <f>RANK(J25,J$2:J$25)</f>
-        <v>24</v>
+        <f t="shared" si="3"/>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J25">
-    <sortState ref="A2:J25">
-      <sortCondition descending="1" ref="J1:J25"/>
+  <autoFilter ref="A1:G25" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState ref="A2:G25">
+      <sortCondition ref="A1:A25"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2472,10 +2131,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
@@ -2580,27 +2239,27 @@
         <v>0.65272940808660596</v>
       </c>
       <c r="L2">
-        <f>RANK(E2,E$2:E$20)</f>
+        <f t="shared" ref="L2:L20" si="0">RANK(E2,E$2:E$20)</f>
         <v>1</v>
       </c>
       <c r="M2">
-        <f>RANK(F2,F$2:F$20)</f>
+        <f t="shared" ref="M2:M20" si="1">RANK(F2,F$2:F$20)</f>
         <v>1</v>
       </c>
       <c r="N2">
-        <f>RANK(G2,G$2:G$20)</f>
+        <f t="shared" ref="N2:N20" si="2">RANK(G2,G$2:G$20)</f>
         <v>19</v>
       </c>
       <c r="O2">
-        <f>RANK(H2,H$2:H$20)</f>
+        <f t="shared" ref="O2:O20" si="3">RANK(H2,H$2:H$20)</f>
         <v>19</v>
       </c>
       <c r="P2">
-        <f>RANK(I2,I$2:I$20)</f>
+        <f t="shared" ref="P2:P20" si="4">RANK(I2,I$2:I$20)</f>
         <v>19</v>
       </c>
       <c r="Q2">
-        <f>RANK(J2,J$2:J$20)</f>
+        <f t="shared" ref="Q2:Q20" si="5">RANK(J2,J$2:J$20)</f>
         <v>19</v>
       </c>
     </row>
@@ -2636,27 +2295,27 @@
         <v>0.82201958970682698</v>
       </c>
       <c r="L3">
-        <f>RANK(E3,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="M3">
-        <f>RANK(F3,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
       <c r="N3">
-        <f>RANK(G3,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
       <c r="O3">
-        <f>RANK(H3,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>18</v>
       </c>
       <c r="P3">
-        <f>RANK(I3,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>8</v>
       </c>
       <c r="Q3">
-        <f>RANK(J3,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>17</v>
       </c>
     </row>
@@ -2692,27 +2351,27 @@
         <v>0.85759943709418895</v>
       </c>
       <c r="L4">
-        <f>RANK(E4,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
       <c r="M4">
-        <f>RANK(F4,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>3</v>
       </c>
       <c r="N4">
-        <f>RANK(G4,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="O4">
-        <f>RANK(H4,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>14</v>
       </c>
       <c r="P4">
-        <f>RANK(I4,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>10</v>
       </c>
       <c r="Q4">
-        <f>RANK(J4,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>15</v>
       </c>
     </row>
@@ -2748,27 +2407,27 @@
         <v>0.86188337820847605</v>
       </c>
       <c r="L5">
-        <f>RANK(E5,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="M5">
-        <f>RANK(F5,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>7</v>
       </c>
       <c r="N5">
-        <f>RANK(G5,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>11</v>
       </c>
       <c r="O5">
-        <f>RANK(H5,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>15</v>
       </c>
       <c r="P5">
-        <f>RANK(I5,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
       <c r="Q5">
-        <f>RANK(J5,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>14</v>
       </c>
     </row>
@@ -2804,27 +2463,27 @@
         <v>0.83021673064214496</v>
       </c>
       <c r="L6">
-        <f>RANK(E6,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="M6">
-        <f>RANK(F6,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>5</v>
       </c>
       <c r="N6">
-        <f>RANK(G6,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="O6">
-        <f>RANK(H6,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>16</v>
       </c>
       <c r="P6">
-        <f>RANK(I6,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>9</v>
       </c>
       <c r="Q6">
-        <f>RANK(J6,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>16</v>
       </c>
     </row>
@@ -2860,27 +2519,27 @@
         <v>0.81138388242761605</v>
       </c>
       <c r="L7">
-        <f>RANK(E7,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="M7">
-        <f>RANK(F7,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>4</v>
       </c>
       <c r="N7">
-        <f>RANK(G7,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>17</v>
       </c>
       <c r="O7">
-        <f>RANK(H7,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>17</v>
       </c>
       <c r="P7">
-        <f>RANK(I7,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>13</v>
       </c>
       <c r="Q7">
-        <f>RANK(J7,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>18</v>
       </c>
     </row>
@@ -2916,27 +2575,27 @@
         <v>1</v>
       </c>
       <c r="L8">
-        <f>RANK(E8,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="M8">
-        <f>RANK(F8,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="N8">
-        <f>RANK(G8,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>5</v>
       </c>
       <c r="O8">
-        <f>RANK(H8,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="P8">
-        <f>RANK(I8,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>5</v>
       </c>
       <c r="Q8">
-        <f>RANK(J8,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>1</v>
       </c>
     </row>
@@ -2972,27 +2631,27 @@
         <v>0.99047514291911398</v>
       </c>
       <c r="L9">
-        <f>RANK(E9,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="M9">
-        <f>RANK(F9,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>8</v>
       </c>
       <c r="N9">
-        <f>RANK(G9,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>4</v>
       </c>
       <c r="O9">
-        <f>RANK(H9,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="P9">
-        <f>RANK(I9,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>4</v>
       </c>
       <c r="Q9">
-        <f>RANK(J9,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
     </row>
@@ -3028,27 +2687,27 @@
         <v>0.94554571947024701</v>
       </c>
       <c r="L10">
-        <f>RANK(E10,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="M10">
-        <f>RANK(F10,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="N10">
-        <f>RANK(G10,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>3</v>
       </c>
       <c r="O10">
-        <f>RANK(H10,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>7</v>
       </c>
       <c r="P10">
-        <f>RANK(I10,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
       <c r="Q10">
-        <f>RANK(J10,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>6</v>
       </c>
     </row>
@@ -3084,27 +2743,27 @@
         <v>0.93677498396412795</v>
       </c>
       <c r="L11">
-        <f>RANK(E11,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="M11">
-        <f>RANK(F11,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="N11">
-        <f>RANK(G11,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>2</v>
       </c>
       <c r="O11">
-        <f>RANK(H11,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>10</v>
       </c>
       <c r="P11">
-        <f>RANK(I11,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="Q11">
-        <f>RANK(J11,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>8</v>
       </c>
     </row>
@@ -3140,27 +2799,27 @@
         <v>0.934563693014834</v>
       </c>
       <c r="L12">
-        <f>RANK(E12,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="M12">
-        <f>RANK(F12,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
       <c r="N12">
-        <f>RANK(G12,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="O12">
-        <f>RANK(H12,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>11</v>
       </c>
       <c r="P12">
-        <f>RANK(I12,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
       <c r="Q12">
-        <f>RANK(J12,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>9</v>
       </c>
     </row>
@@ -3196,27 +2855,27 @@
         <v>0.91117878510690797</v>
       </c>
       <c r="L13">
-        <f>RANK(E13,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="M13">
-        <f>RANK(F13,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="N13">
-        <f>RANK(G13,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
       <c r="O13">
-        <f>RANK(H13,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="P13">
-        <f>RANK(I13,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>6</v>
       </c>
       <c r="Q13">
-        <f>RANK(J13,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
     </row>
@@ -3252,27 +2911,27 @@
         <v>0.87633037392801605</v>
       </c>
       <c r="L14">
-        <f>RANK(E14,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="M14">
-        <f>RANK(F14,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="N14">
-        <f>RANK(G14,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>13</v>
       </c>
       <c r="O14">
-        <f>RANK(H14,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>13</v>
       </c>
       <c r="P14">
-        <f>RANK(I14,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
       <c r="Q14">
-        <f>RANK(J14,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>13</v>
       </c>
     </row>
@@ -3308,27 +2967,27 @@
         <v>0.94984115085023901</v>
       </c>
       <c r="L15">
-        <f>RANK(E15,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="M15">
-        <f>RANK(F15,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="N15">
-        <f>RANK(G15,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>10</v>
       </c>
       <c r="O15">
-        <f>RANK(H15,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>3</v>
       </c>
       <c r="P15">
-        <f>RANK(I15,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="Q15">
-        <f>RANK(J15,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>3</v>
       </c>
     </row>
@@ -3364,27 +3023,27 @@
         <v>0.94751581682763197</v>
       </c>
       <c r="L16">
-        <f>RANK(E16,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="M16">
-        <f>RANK(F16,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
       <c r="N16">
-        <f>RANK(G16,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="O16">
-        <f>RANK(H16,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P16">
-        <f>RANK(I16,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="Q16">
-        <f>RANK(J16,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -3420,27 +3079,27 @@
         <v>0.94751581682763197</v>
       </c>
       <c r="L17">
-        <f>RANK(E17,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="M17">
-        <f>RANK(F17,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
       <c r="N17">
-        <f>RANK(G17,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>8</v>
       </c>
       <c r="O17">
-        <f>RANK(H17,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
       <c r="P17">
-        <f>RANK(I17,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>14</v>
       </c>
       <c r="Q17">
-        <f>RANK(J17,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -3476,27 +3135,27 @@
         <v>0.94539557869122604</v>
       </c>
       <c r="L18">
-        <f>RANK(E18,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="M18">
-        <f>RANK(F18,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="N18">
-        <f>RANK(G18,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
       <c r="O18">
-        <f>RANK(H18,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>6</v>
       </c>
       <c r="P18">
-        <f>RANK(I18,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>11</v>
       </c>
       <c r="Q18">
-        <f>RANK(J18,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>7</v>
       </c>
     </row>
@@ -3532,27 +3191,27 @@
         <v>0.922314295624169</v>
       </c>
       <c r="L19">
-        <f>RANK(E19,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="M19">
-        <f>RANK(F19,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
       <c r="N19">
-        <f>RANK(G19,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>14</v>
       </c>
       <c r="O19">
-        <f>RANK(H19,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>9</v>
       </c>
       <c r="P19">
-        <f>RANK(I19,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
       <c r="Q19">
-        <f>RANK(J19,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
     </row>
@@ -3588,32 +3247,32 @@
         <v>0.92978725591212896</v>
       </c>
       <c r="L20">
-        <f>RANK(E20,E$2:E$20)</f>
+        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="M20">
-        <f>RANK(F20,F$2:F$20)</f>
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
       <c r="N20">
-        <f>RANK(G20,G$2:G$20)</f>
+        <f t="shared" si="2"/>
         <v>12</v>
       </c>
       <c r="O20">
-        <f>RANK(H20,H$2:H$20)</f>
+        <f t="shared" si="3"/>
         <v>8</v>
       </c>
       <c r="P20">
-        <f>RANK(I20,I$2:I$20)</f>
+        <f t="shared" si="4"/>
         <v>17</v>
       </c>
       <c r="Q20">
-        <f>RANK(J20,J$2:J$20)</f>
+        <f t="shared" si="5"/>
         <v>10</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:Q31">
+  <autoFilter ref="A1:Q31" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState ref="A2:Q31">
       <sortCondition descending="1" ref="E1:E31"/>
     </sortState>

</xml_diff>